<commit_message>
Project 3: RPC Proxy Hello World
</commit_message>
<xml_diff>
--- a/project2/Results2.xlsx
+++ b/project2/Results2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="208" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="208" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Centralized" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>Centralized OMP</t>
   </si>
@@ -59,6 +59,12 @@
     <t>Number of Pr</t>
   </si>
   <si>
+    <t>Cent MPI</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
     <t>Process</t>
   </si>
   <si>
@@ -75,9 +81,6 @@
   </si>
   <si>
     <t>Barriers</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -272,19 +275,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I238"/>
+  <dimension ref="A2:K238"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H31" activeCellId="0" pane="topLeft" sqref="H31"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K26" activeCellId="0" pane="topLeft" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
@@ -331,6 +334,12 @@
       <c r="H5" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="J5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="D6" s="0" t="n">
@@ -345,6 +354,12 @@
       <c r="H6" s="0" t="n">
         <v>232</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="D7" s="1" t="s">
@@ -359,6 +374,12 @@
       <c r="H7" s="0" t="n">
         <v>451</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>252</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="D8" s="0" t="n">
@@ -375,6 +396,9 @@
       </c>
       <c r="I8" s="0" t="n">
         <v>780</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -516,6 +540,12 @@
       <c r="H25" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
@@ -532,6 +562,9 @@
       </c>
       <c r="H26" s="4" t="n">
         <v>580</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
@@ -549,6 +582,9 @@
         <f aca="false">SUM(E47+E53+E59+E65+E71)/5</f>
         <v>891.25</v>
       </c>
+      <c r="J27" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="G28" s="0" t="n">
@@ -556,7 +592,10 @@
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">SUM(E80,E87,E94)/3</f>
-        <v>1260.35555555556</v>
+        <v>1260.35555555555</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
@@ -570,6 +609,9 @@
         <f aca="false">SUM(E112,E121,E130,E103, E139)/5</f>
         <v>1383.675</v>
       </c>
+      <c r="J29" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="G30" s="0" t="n">
@@ -579,6 +621,9 @@
         <f aca="false">SUM(E151,E162,E173,E184)/4</f>
         <v>1964.725</v>
       </c>
+      <c r="J30" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="G31" s="0" t="n">
@@ -587,6 +632,9 @@
       <c r="H31" s="1" t="n">
         <f aca="false">SUM(E199,E212,E238)/3</f>
         <v>2146.33333333333</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
@@ -2167,27 +2215,27 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -2207,7 +2255,7 @@
         <v>245</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="C3" s="0" t="n">
         <v>249</v>
       </c>
@@ -2221,7 +2269,7 @@
         <v>618</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="C4" s="1" t="n">
         <f aca="false">SUM(C2:C3)/2</f>
         <v>245.5</v>
@@ -2236,7 +2284,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="E5" s="0" t="n">
         <v>2</v>
       </c>
@@ -2248,7 +2296,7 @@
         <v>2099.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>2</v>
       </c>
@@ -2259,7 +2307,7 @@
         <v>621</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="C7" s="0" t="n">
         <v>616</v>
       </c>
@@ -2274,7 +2322,7 @@
         <v>359</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="C8" s="1" t="n">
         <f aca="false">SUM(C6:C7)/2</f>
         <v>618.5</v>
@@ -2290,7 +2338,7 @@
         <v>747</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="E9" s="0" t="n">
         <v>4</v>
       </c>
@@ -2302,7 +2350,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
@@ -2323,12 +2371,12 @@
         <v>2105.75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="C11" s="0" t="n">
         <v>1352</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="C12" s="1" t="n">
         <f aca="false">SUM(C10:C11)/2</f>
         <v>1354</v>
@@ -2344,7 +2392,7 @@
         <v>405</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="E13" s="0" t="n">
         <v>6</v>
       </c>
@@ -2356,7 +2404,7 @@
         <v>826</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>2</v>
       </c>
@@ -2377,7 +2425,7 @@
         <v>1570.66666666667</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="C15" s="0" t="n">
         <v>2102</v>
       </c>
@@ -2392,8 +2440,8 @@
         <v>2164.66666666667</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>4</v>
       </c>
@@ -2410,7 +2458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="C18" s="0" t="n">
         <v>362</v>
       </c>
@@ -2421,7 +2469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="C19" s="0" t="n">
         <v>363</v>
       </c>
@@ -2432,7 +2480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="C20" s="0" t="n">
         <v>351</v>
       </c>
@@ -2443,8 +2491,8 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>4</v>
       </c>
@@ -2455,24 +2503,24 @@
         <v>750</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="C23" s="0" t="n">
         <v>750</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="C24" s="0" t="n">
         <v>739</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="C25" s="0" t="n">
         <v>749</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>4</v>
       </c>
@@ -2483,23 +2531,23 @@
         <v>1502</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="C29" s="0" t="n">
         <v>1504</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="C30" s="0" t="n">
         <v>1503</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="C31" s="0" t="n">
         <v>1491</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>4</v>
       </c>
@@ -2510,24 +2558,24 @@
         <v>2109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="C35" s="0" t="n">
         <v>2109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="C36" s="0" t="n">
         <v>2097</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="C37" s="0" t="n">
         <v>2108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
         <v>6</v>
       </c>
@@ -2538,33 +2586,33 @@
         <v>407</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="C41" s="0" t="n">
         <v>408</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="C42" s="0" t="n">
         <v>409</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="C43" s="0" t="n">
         <v>406</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="C44" s="0" t="n">
         <v>407</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="C45" s="0" t="n">
         <v>393</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>6</v>
       </c>
@@ -2575,32 +2623,32 @@
         <v>829</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="C49" s="0" t="n">
         <v>831</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="C50" s="0" t="n">
         <v>828</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="C51" s="0" t="n">
         <v>814</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="C52" s="0" t="n">
         <v>824</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="C53" s="0" t="n">
         <v>830</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
         <v>6</v>
       </c>
@@ -2611,32 +2659,32 @@
         <v>1571</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="C57" s="0" t="n">
         <v>1573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="C58" s="0" t="n">
         <v>1581</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="C59" s="0" t="n">
         <v>1570</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="C60" s="0" t="n">
         <v>1556</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="C61" s="0" t="n">
         <v>1573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
         <v>6</v>
       </c>
@@ -2647,32 +2695,32 @@
         <v>2168</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="C64" s="0" t="n">
         <v>2152</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="C65" s="0" t="n">
         <v>2169</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="C66" s="0" t="n">
         <v>2166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="C67" s="0" t="n">
         <v>2166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="C68" s="0" t="n">
         <v>2167</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
         <v>8</v>
       </c>
@@ -2683,42 +2731,42 @@
         <v>430</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="C71" s="0" t="n">
         <v>416</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="C72" s="0" t="n">
         <v>428</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="C73" s="0" t="n">
         <v>431</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="C74" s="0" t="n">
         <v>429</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="C75" s="0" t="n">
         <v>432</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="C76" s="0" t="n">
         <v>430</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="C77" s="0" t="n">
         <v>427</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="n">
         <v>8</v>
       </c>
@@ -2729,42 +2777,42 @@
         <v>867</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="C80" s="0" t="n">
         <v>848</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="C81" s="0" t="n">
         <v>859</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="C82" s="0" t="n">
         <v>858</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="C83" s="0" t="n">
         <v>861</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="C84" s="0" t="n">
         <v>861</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="C85" s="0" t="n">
         <v>861</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="C86" s="0" t="n">
         <v>860</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="n">
         <v>8</v>
       </c>
@@ -2775,43 +2823,43 @@
         <v>1634</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="C89" s="0" t="n">
         <v>1616</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="C90" s="0" t="n">
         <v>1626</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="91">
       <c r="C91" s="0" t="n">
         <v>1625</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="C92" s="0" t="n">
         <v>1626</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="93">
       <c r="C93" s="0" t="n">
         <v>1626</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="C94" s="0" t="n">
         <v>1625</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="C95" s="0" t="n">
         <v>1628</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="96"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="A98" s="0" t="n">
         <v>8</v>
       </c>
@@ -2831,6 +2879,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2855,31 +2928,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2887,31 +2935,31 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -2919,7 +2967,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
@@ -2927,7 +2975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>6</v>
       </c>
@@ -2935,7 +2983,7 @@
         <v>104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>8</v>
       </c>
@@ -2966,7 +3014,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2991,7 +3039,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>